<commit_message>
updates tables with new queries and validates xml
</commit_message>
<xml_diff>
--- a/data-raw/DeltaEntry_RecapturesRaw.xlsx
+++ b/data-raw/DeltaEntry_RecapturesRaw.xlsx
@@ -67,11 +67,6 @@
       <color rgb="FF000000" tint="0"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000" tint="0"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -90,12 +85,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC0C0C0"/>
         <bgColor rgb="FFC0C0C0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -148,20 +137,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFD0D7E5"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFD0D7E5"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFD0D7E5"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFD0D7E5"/>
-      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -277,15 +252,11 @@
       <alignment wrapText="1" vertical="center" horizontal="general"/>
       <protection locked="1" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" applyFill="1" applyProtection="1" applyBorder="1" applyAlignment="1" applyFont="1" xfId="0">
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="6" applyFill="1" applyProtection="1" applyBorder="1" applyAlignment="1" applyNumberFormat="1" applyFont="1" xfId="0">
       <alignment wrapText="1" vertical="center" horizontal="right"/>
       <protection locked="1" hidden="0"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="9" borderId="7" applyFill="1" applyProtection="1" applyBorder="1" applyAlignment="1" applyNumberFormat="1" applyFont="1" xfId="0">
-      <alignment wrapText="1" vertical="center" horizontal="right"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" applyFill="1" applyProtection="1" applyBorder="1" applyAlignment="1" applyFont="1" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="7" applyFill="1" applyProtection="1" applyBorder="1" applyAlignment="1" applyFont="1" xfId="0">
       <alignment wrapText="1" vertical="center" horizontal="general"/>
       <protection locked="1" hidden="0"/>
     </xf>
@@ -583,7 +554,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -601,19 +572,16 @@
     <col customWidth="true" min="8" max="8" width="19.921875"/>
     <col customWidth="true" min="9" max="9" width="36.03515625"/>
     <col customWidth="true" min="10" max="10" width="19.921875"/>
-    <col customWidth="true" min="11" max="11" width="19.921875"/>
-    <col customWidth="true" min="12" max="12" width="13.9140625"/>
-    <col customWidth="true" min="13" max="13" width="14.5"/>
-    <col customWidth="true" min="14" max="14" width="13.62109375"/>
-    <col customWidth="true" min="15" max="15" width="16.84375"/>
-    <col customWidth="true" min="16" max="16" width="22.265625"/>
-    <col customWidth="true" min="17" max="17" width="74.12109375"/>
-    <col customWidth="true" min="18" max="18" width="38.96484375"/>
-    <col customWidth="true" min="19" max="19" width="16.2578125"/>
-    <col customWidth="true" min="20" max="20" width="22.1171875"/>
-    <col customWidth="true" min="21" max="21" width="19.921875"/>
-    <col customWidth="true" min="22" max="22" width="30.76171875"/>
-    <col customWidth="true" min="23" max="23" width="13.328125"/>
+    <col customWidth="true" min="11" max="11" width="13.9140625"/>
+    <col customWidth="true" min="12" max="12" width="14.5"/>
+    <col customWidth="true" min="13" max="13" width="13.62109375"/>
+    <col customWidth="true" min="14" max="14" width="22.265625"/>
+    <col customWidth="true" min="15" max="15" width="74.12109375"/>
+    <col customWidth="true" min="16" max="16" width="38.96484375"/>
+    <col customWidth="true" min="17" max="17" width="16.2578125"/>
+    <col customWidth="true" min="18" max="18" width="22.1171875"/>
+    <col customWidth="true" min="19" max="19" width="19.921875"/>
+    <col customWidth="true" min="20" max="20" width="30.76171875"/>
   </cols>
   <sheetData>
     <row outlineLevel="0" r="1">
@@ -664,72 +632,57 @@
       </c>
       <c r="J1" s="2" t="inlineStr">
         <is>
-          <t>mort</t>
+          <t>actualCount</t>
         </is>
       </c>
       <c r="K1" s="2" t="inlineStr">
         <is>
-          <t>actualCount</t>
+          <t>forkLength</t>
         </is>
       </c>
       <c r="L1" s="2" t="inlineStr">
         <is>
-          <t>forkLength</t>
+          <t>totalLength</t>
         </is>
       </c>
       <c r="M1" s="2" t="inlineStr">
         <is>
-          <t>totalLength</t>
+          <t>n</t>
         </is>
       </c>
       <c r="N1" s="2" t="inlineStr">
         <is>
-          <t>n</t>
+          <t>visitTime</t>
         </is>
       </c>
       <c r="O1" s="2" t="inlineStr">
         <is>
-          <t>actualCountID</t>
+          <t>visitType</t>
         </is>
       </c>
       <c r="P1" s="2" t="inlineStr">
         <is>
-          <t>visitTime</t>
+          <t>siteName</t>
         </is>
       </c>
       <c r="Q1" s="2" t="inlineStr">
         <is>
-          <t>visitType</t>
+          <t>subSiteName</t>
         </is>
       </c>
       <c r="R1" s="2" t="inlineStr">
         <is>
-          <t>siteName</t>
+          <t>markType</t>
         </is>
       </c>
       <c r="S1" s="2" t="inlineStr">
         <is>
-          <t>subSiteName</t>
+          <t>markColor</t>
         </is>
       </c>
       <c r="T1" s="2" t="inlineStr">
         <is>
-          <t>markType</t>
-        </is>
-      </c>
-      <c r="U1" s="2" t="inlineStr">
-        <is>
-          <t>markColor</t>
-        </is>
-      </c>
-      <c r="V1" s="2" t="inlineStr">
-        <is>
           <t>markPosition</t>
-        </is>
-      </c>
-      <c r="W1" s="2" t="inlineStr">
-        <is>
-          <t>markCode</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
removes NAs from recapture table
</commit_message>
<xml_diff>
--- a/data-raw/DeltaEntry_RecapturesRaw.xlsx
+++ b/data-raw/DeltaEntry_RecapturesRaw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-delta-entry-edi/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CB80B7-FD8D-8E4B-9A69-18C1B3727D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E2C632-02F5-8942-B5FB-7CAE8AE3067C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="760" windowWidth="23900" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ProjectDescriptionID</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>markPosition</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -158,7 +155,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -554,66 +551,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>